<commit_message>
Push dei dati (nome, cognome, iban)
</commit_message>
<xml_diff>
--- a/Excel/File/Output/output.xlsx
+++ b/Excel/File/Output/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,21 +441,340 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nanni</t>
+          <t xml:space="preserve"> Franco</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Dallara</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT22G0911802828638328716550</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Massimo</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bragadin</t>
+          <t xml:space="preserve"> Ponti</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT18W8034292104481328055001</t>
         </is>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Donato</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Berrï¿½</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IT47V9390981684727103408033</t>
+          <t xml:space="preserve"> IT46C0861777507940288399049</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Irma</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Grossi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT52Y0357680245497703784766</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Alessia</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Inzaghi</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT87S3236428872725803131321</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fernanda</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Castellitto</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT77G0817953418013202089394</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Achille</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Balotelli</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT21A8964054634106625019577</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Giorgio</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Alighieri</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT14J1519202636883865277705</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Antonina</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Faranda</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT07Q5630412441332153455987</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Rosario</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Segni</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT38O7106928503256334884185</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gastone</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bernardini</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT24X2658564212392332035647</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Coluccio</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Viviani</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT06V7548083700894609986605</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gabriella</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Varano</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT03V2159643755478463515322</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pomponio</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Quasimodo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT62Z0418512675125175253843</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ugolino</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tomasini</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT46K5437180682756522779430</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bianca</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bongiorno</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT33Q5910847349340989270366</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Micheletto</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Renzi</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT92X9428267733656148257548</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Benedetto</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Federici</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT45J6523854350322959056872</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Domenico</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Barese</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT14Y5014754707952219213232</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nanni</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bragadin</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT47V9390981684727103408033</t>
         </is>
       </c>
     </row>

</xml_diff>